<commit_message>
DMS: Fix Store and StoreScouting import
</commit_message>
<xml_diff>
--- a/DMS/Templates/StoreScouting_Template.xlsx
+++ b/DMS/Templates/StoreScouting_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\dotNet\DMS\DMS.BE\DMS\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C37E0AB3-C843-4290-9C56-94A6CA1F3CF5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{201A4ED1-A9EA-41E1-842A-ACB4CD4F3F4B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Đại lý cắm cờ" sheetId="1" r:id="rId1"/>
@@ -512,7 +512,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
@@ -606,7 +606,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>

</xml_diff>